<commit_message>
fast commit @ 2024/05/12 周日 20:02:08.28
</commit_message>
<xml_diff>
--- a/学校课程笔记/荐购书单.xlsx
+++ b/学校课程笔记/荐购书单.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git_repository\Notes\学校课程笔记\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33107\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92F317E-DD5B-4F49-A96A-1DD6B872CF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB64E1-B244-429D-B04E-8CD2158E231F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-8168" windowWidth="28995" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>枪炮病菌与钢铁</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -377,6 +377,46 @@
   </si>
   <si>
     <t>八次危机：中国的真实经验</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《on writing well》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《详解FPGA：人工智能时代的驱动引擎》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《数字VLSI芯片设计：使用Cadence和Synopsys CAD工具》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《模拟CMOS集成电路设计》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《千年一叹》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《明朝那些事儿》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《我与地坛》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《三体》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《查理九世》</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>《SystemVerilog验证：测试平台编写指南》</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -745,22 +785,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.88671875" customWidth="1"/>
-    <col min="2" max="2" width="59.6640625" customWidth="1"/>
-    <col min="3" max="3" width="64.33203125" customWidth="1"/>
-    <col min="4" max="4" width="63.21875" customWidth="1"/>
-    <col min="7" max="7" width="55.77734375" customWidth="1"/>
+    <col min="1" max="1" width="48.875" customWidth="1"/>
+    <col min="2" max="2" width="59.625" customWidth="1"/>
+    <col min="3" max="3" width="64.375" customWidth="1"/>
+    <col min="4" max="4" width="63.25" customWidth="1"/>
+    <col min="7" max="7" width="55.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -774,7 +814,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -788,7 +828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -799,7 +839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -810,7 +850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -821,7 +861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -832,7 +872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -843,7 +883,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -854,7 +894,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -865,7 +905,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -876,7 +916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -887,7 +927,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -898,7 +938,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -909,7 +949,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -920,7 +960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -931,7 +971,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -942,7 +982,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -953,7 +993,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -964,7 +1004,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -975,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -986,7 +1026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -997,7 +1037,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1008,7 +1048,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -1019,7 +1059,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1030,7 +1070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -1041,7 +1081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1052,7 +1092,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1063,7 +1103,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1074,7 +1114,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1082,47 +1122,62 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>83</v>
       </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
       <c r="C30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>84</v>
       </c>
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
       <c r="C31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>85</v>
       </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
       <c r="C32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>86</v>
       </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
       <c r="C33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>87</v>
       </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
       <c r="C34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -1130,7 +1185,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -1138,29 +1193,54 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>